<commit_message>
Adds Master Test Plan
</commit_message>
<xml_diff>
--- a/QA files/Test Plan.xlsx
+++ b/QA files/Test Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgiev\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgiev\Documents\Github\Damwon\QA files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite 1" sheetId="1" r:id="rId1"/>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +976,7 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1217,7 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>